<commit_message>
bug fixing making a game work fully
</commit_message>
<xml_diff>
--- a/UndyingBuddies/Assets/EquilibrageUndyingBuddies.xlsx
+++ b/UndyingBuddies/Assets/EquilibrageUndyingBuddies.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Unity\UndyingBuddies\UndyingBuddies\UndyingBuddies\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEE83DC7-8A06-47C6-9137-61C5E7689B27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9D56DC3-A12F-4E15-9AE3-74810B6B68B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{B2102F43-0C7C-4931-8CF5-294E0545DE19}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{B2102F43-0C7C-4931-8CF5-294E0545DE19}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil2" sheetId="3" r:id="rId1"/>
     <sheet name="Feuil3" sheetId="4" r:id="rId2"/>
     <sheet name="Crystals" sheetId="5" r:id="rId3"/>
+    <sheet name="ItemValue" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="63">
   <si>
     <t>tree</t>
   </si>
@@ -179,14 +180,67 @@
   </si>
   <si>
     <t>energy / sec</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>BrokenSoul</t>
+  </si>
+  <si>
+    <t>WhiteSoul</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>BlueVioletSoult</t>
+  </si>
+  <si>
+    <t>VioletSoul</t>
+  </si>
+  <si>
+    <t>BlueSoul</t>
+  </si>
+  <si>
+    <t>RedSoul</t>
+  </si>
+  <si>
+    <t>ItemName</t>
+  </si>
+  <si>
+    <t>input 1</t>
+  </si>
+  <si>
+    <t>input 1 name</t>
+  </si>
+  <si>
+    <t>input 1 value</t>
+  </si>
+  <si>
+    <t>nothing</t>
+  </si>
+  <si>
+    <t>RealValue</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -214,8 +268,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1176,15 +1231,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6A1CD48-9B98-4267-9514-47E1C43D74E3}">
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U19" sqref="U19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -1464,6 +1524,363 @@
         <v>9</v>
       </c>
     </row>
+    <row r="18" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K18" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19" t="str">
+        <f>INDEX(ItemValue!B:B,MATCH(Crystals!A19,ItemValue!A:A))</f>
+        <v>WhiteSoul</v>
+      </c>
+      <c r="C19">
+        <f>INDEX(ItemValue!C:C,MATCH(Crystals!A19,ItemValue!A:A))</f>
+        <v>3</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19" t="str">
+        <f>INDEX(ItemValue!B:B,MATCH(Crystals!D19,ItemValue!A:A))</f>
+        <v>BrokenSoul</v>
+      </c>
+      <c r="F19">
+        <f>INDEX(ItemValue!C:C,MATCH(Crystals!D19,ItemValue!A:A))</f>
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>6</v>
+      </c>
+      <c r="H19" t="str">
+        <f>INDEX(ItemValue!B:B,MATCH(Crystals!G19,ItemValue!A:A))</f>
+        <v>nothing</v>
+      </c>
+      <c r="I19">
+        <f>INDEX(ItemValue!C:C,MATCH(Crystals!G19,ItemValue!A:A))</f>
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <f>C19-F19-I19</f>
+        <v>2</v>
+      </c>
+      <c r="K19">
+        <f>J19/K18</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20" t="str">
+        <f>INDEX(ItemValue!B:B,MATCH(Crystals!A20,ItemValue!A:A))</f>
+        <v>BlueVioletSoult</v>
+      </c>
+      <c r="C20">
+        <f>INDEX(ItemValue!C:C,MATCH(Crystals!A20,ItemValue!A:A))</f>
+        <v>7</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" t="str">
+        <f>INDEX(ItemValue!B:B,MATCH(Crystals!D20,ItemValue!A:A))</f>
+        <v>WhiteSoul</v>
+      </c>
+      <c r="F20">
+        <f>INDEX(ItemValue!C:C,MATCH(Crystals!D20,ItemValue!A:A))</f>
+        <v>3</v>
+      </c>
+      <c r="G20">
+        <v>6</v>
+      </c>
+      <c r="H20" t="str">
+        <f>INDEX(ItemValue!B:B,MATCH(Crystals!G20,ItemValue!A:A))</f>
+        <v>nothing</v>
+      </c>
+      <c r="I20">
+        <f>INDEX(ItemValue!C:C,MATCH(Crystals!G20,ItemValue!A:A))</f>
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <f>C20-F20-I20</f>
+        <v>4</v>
+      </c>
+      <c r="K20">
+        <f>J20/J19</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>3</v>
+      </c>
+      <c r="B21" t="str">
+        <f>INDEX(ItemValue!B:B,MATCH(Crystals!A21,ItemValue!A:A))</f>
+        <v>VioletSoul</v>
+      </c>
+      <c r="C21">
+        <f>INDEX(ItemValue!C:C,MATCH(Crystals!A21,ItemValue!A:A))</f>
+        <v>18</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" t="str">
+        <f>INDEX(ItemValue!B:B,MATCH(Crystals!D21,ItemValue!A:A))</f>
+        <v>WhiteSoul</v>
+      </c>
+      <c r="F21">
+        <f>INDEX(ItemValue!C:C,MATCH(Crystals!D21,ItemValue!A:A))</f>
+        <v>3</v>
+      </c>
+      <c r="G21">
+        <v>2</v>
+      </c>
+      <c r="H21" t="str">
+        <f>INDEX(ItemValue!B:B,MATCH(Crystals!G21,ItemValue!A:A))</f>
+        <v>BlueVioletSoult</v>
+      </c>
+      <c r="I21">
+        <f>INDEX(ItemValue!C:C,MATCH(Crystals!G21,ItemValue!A:A))</f>
+        <v>7</v>
+      </c>
+      <c r="J21">
+        <f>C21-F21-I21</f>
+        <v>8</v>
+      </c>
+      <c r="K21">
+        <f>J21/J20</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>4</v>
+      </c>
+      <c r="B22" t="str">
+        <f>INDEX(ItemValue!B:B,MATCH(Crystals!A22,ItemValue!A:A))</f>
+        <v>BlueSoul</v>
+      </c>
+      <c r="C22">
+        <f>INDEX(ItemValue!C:C,MATCH(Crystals!A22,ItemValue!A:A))</f>
+        <v>37</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22" t="str">
+        <f>INDEX(ItemValue!B:B,MATCH(Crystals!D22,ItemValue!A:A))</f>
+        <v>WhiteSoul</v>
+      </c>
+      <c r="F22">
+        <f>INDEX(ItemValue!C:C,MATCH(Crystals!D22,ItemValue!A:A))</f>
+        <v>3</v>
+      </c>
+      <c r="G22">
+        <v>3</v>
+      </c>
+      <c r="H22" t="str">
+        <f>INDEX(ItemValue!B:B,MATCH(Crystals!G22,ItemValue!A:A))</f>
+        <v>VioletSoul</v>
+      </c>
+      <c r="I22">
+        <f>INDEX(ItemValue!C:C,MATCH(Crystals!G22,ItemValue!A:A))</f>
+        <v>18</v>
+      </c>
+      <c r="J22">
+        <f>C22-F22-I22</f>
+        <v>16</v>
+      </c>
+      <c r="K22">
+        <f>J22/J21</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>5</v>
+      </c>
+      <c r="B23" t="str">
+        <f>INDEX(ItemValue!B:B,MATCH(Crystals!A23,ItemValue!A:A))</f>
+        <v>RedSoul</v>
+      </c>
+      <c r="C23">
+        <f>INDEX(ItemValue!C:C,MATCH(Crystals!A23,ItemValue!A:A))</f>
+        <v>57</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+      <c r="E23" t="str">
+        <f>INDEX(ItemValue!B:B,MATCH(Crystals!D23,ItemValue!A:A))</f>
+        <v>BlueVioletSoult</v>
+      </c>
+      <c r="F23">
+        <f>INDEX(ItemValue!C:C,MATCH(Crystals!D23,ItemValue!A:A))</f>
+        <v>7</v>
+      </c>
+      <c r="G23">
+        <v>3</v>
+      </c>
+      <c r="H23" t="str">
+        <f>INDEX(ItemValue!B:B,MATCH(Crystals!G23,ItemValue!A:A))</f>
+        <v>VioletSoul</v>
+      </c>
+      <c r="I23">
+        <f>INDEX(ItemValue!C:C,MATCH(Crystals!G23,ItemValue!A:A))</f>
+        <v>18</v>
+      </c>
+      <c r="J23">
+        <f>C23-F23-I23</f>
+        <v>32</v>
+      </c>
+      <c r="K23">
+        <f>J23/J22</f>
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D14DE2F-7D04-44DF-A1C5-5C8E195FBCCC}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>